<commit_message>
se simplificó la estructura del proyecto
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>TC1</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>C200061452</t>
+  </si>
+  <si>
+    <t>C200061460</t>
   </si>
 </sst>
 </file>
@@ -155,7 +158,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +205,11 @@
       <sz val="11.0"/>
       <color indexed="17"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -235,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -264,7 +272,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -672,7 +681,7 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
se agregó escenario carga de materiales
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>TC1</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>C200061460</t>
+  </si>
+  <si>
+    <t>C200061465</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +213,11 @@
       <sz val="11.0"/>
       <color indexed="17"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -243,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -273,7 +281,8 @@
     </xf>
     <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -681,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
se cambio el nombre de un tag crearpedido
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>TC1</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>C200061465</t>
+  </si>
+  <si>
+    <t>C200061471</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +221,11 @@
       <sz val="11.0"/>
       <color indexed="17"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -251,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -282,7 +290,8 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
     <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -690,7 +699,7 @@
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
actualización LOG feature CreacionPedido
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView windowHeight="2760" windowWidth="14670" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="2760"/>
   </bookViews>
   <sheets>
-    <sheet name="Corporativo" r:id="rId1" sheetId="1"/>
+    <sheet name="Corporativo" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>TC1</t>
   </si>
@@ -138,15 +138,17 @@
     <t>03863301</t>
   </si>
   <si>
-    <t>C200061493</t>
+    <t>Cod_Pedido</t>
+  </si>
+  <si>
+    <t>C200061532</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,13 +185,8 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -219,43 +222,45 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" quotePrefix="1" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -272,10 +277,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -310,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -345,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -439,21 +444,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -470,7 +475,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -522,81 +527,84 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="56.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O1"/>
+      <c r="O1" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -616,267 +624,269 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
     </row>
-    <row customFormat="1" ht="16.5" r="2" s="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:33" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>72477280</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="7">
         <v>72198770</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>72477280</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>2</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="10">
         <v>72198770</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O3"/>
       <c r="AB3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>72477280</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="3">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="10">
         <v>72198770</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="6" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="7" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="8" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="9" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="10" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="11" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="12" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="13" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="14" s="1" spans="1:33" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="15" s="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="E15" s="6" t="s">
+    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row customFormat="1" r="16" s="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="E16" s="5" t="s">
+    <row r="16" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="1" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="5" t="s">
+    <row r="17" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="1" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="5" t="s">
+    <row r="18" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row customFormat="1" r="19" s="1" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="5" t="s">
+    <row r="19" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row customFormat="1" r="20" s="1" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="5" t="s">
+    <row r="20" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row customFormat="1" r="21" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="22" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="23" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="24" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="25" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="26" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="27" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="28" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="29" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="30" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="31" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="32" s="1" spans="5:9" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="33" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="34" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="35" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="36" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="37" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="38" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="39" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="40" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="41" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="42" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="43" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="44" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="45" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="46" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="47" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="48" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="49" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="50" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="51" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="52" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="53" s="1" x14ac:dyDescent="0.25"/>
-    <row customFormat="1" r="54" s="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="5:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G2:G4" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
       <formula1>$G$16:$G$19</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="I2:I4" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I4">
       <formula1>$I$16:$I$17</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="F2:F4" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
       <formula1>$F$16:$F$17</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="E2:E4" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>$E$16:$E$20</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregó feature Carga materiales
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CREACION_PEDIDO.xlsx
+++ b/src/main/resources/excel/CREACION_PEDIDO.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14670" windowHeight="2760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Corporativo" sheetId="1" r:id="rId1"/>
+    <sheet name="Residencial" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>TC1</t>
   </si>
@@ -141,14 +142,29 @@
     <t>Cod_Pedido</t>
   </si>
   <si>
-    <t>C200061532</t>
+    <t>ID_ORDEN</t>
+  </si>
+  <si>
+    <t>IMEI</t>
+  </si>
+  <si>
+    <t>SIMCARD</t>
+  </si>
+  <si>
+    <t>123900000146889</t>
+  </si>
+  <si>
+    <t>123900000146897</t>
+  </si>
+  <si>
+    <t>8958080008100290000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +200,13 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -224,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,14 +268,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -537,14 +566,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="16.140625" customWidth="1" collapsed="1"/>
@@ -624,9 +653,9 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
     </row>
-    <row r="2" spans="1:33" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="3">
@@ -656,25 +685,23 @@
       <c r="K2" s="7">
         <v>72198770</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
+      <c r="O2"/>
       <c r="AB2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="3">
@@ -701,13 +728,13 @@
       <c r="J3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>72198770</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="N3" s="3" t="s">
@@ -717,9 +744,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="3">
@@ -746,13 +773,13 @@
       <c r="J4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>72198770</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="8" t="s">
         <v>28</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -889,4 +916,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="11">
+        <v>72477280</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="11">
+        <v>1090591</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="11">
+        <v>72477280</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1089499</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>